<commit_message>
udpated the structure of lecture 2 part 2
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/jancg_sun_ac_za/Documents/3_LE/3_Courses/AE_772_892/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{1656F390-B7D1-0445-960B-12713EC63637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E0BD4BF-0BE6-8E48-B767-F4DC10518D9E}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{1656F390-B7D1-0445-960B-12713EC63637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C2BBC5D-05B4-2345-AF1F-4FD8B43F442F}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{74ACAC89-5DCE-FD43-9BD5-16FF9C56919D}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{74ACAC89-5DCE-FD43-9BD5-16FF9C56919D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Classlist" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Quizes</t>
   </si>
@@ -156,6 +157,72 @@
   </si>
   <si>
     <t>Max mark</t>
+  </si>
+  <si>
+    <t>Mbongwe,</t>
+  </si>
+  <si>
+    <t>KA,</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>[22639438@sun.ac.za]</t>
+  </si>
+  <si>
+    <t>F,</t>
+  </si>
+  <si>
+    <t>Mnr</t>
+  </si>
+  <si>
+    <t>[22552987@sun.ac.za]</t>
+  </si>
+  <si>
+    <t>Matthysen,</t>
+  </si>
+  <si>
+    <t>LP,</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>[22899537@sun.ac.za]</t>
+  </si>
+  <si>
+    <t>Mofokeng,</t>
+  </si>
+  <si>
+    <t>D,</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>[22309667@sun.ac.za]</t>
+  </si>
+  <si>
+    <t>Schultz,</t>
+  </si>
+  <si>
+    <t>K,</t>
+  </si>
+  <si>
+    <t>[22539026@sun.ac.za]</t>
+  </si>
+  <si>
+    <t>Sinclair,</t>
+  </si>
+  <si>
+    <t>HW,</t>
+  </si>
+  <si>
+    <t>[21672598@sun.ac.za]</t>
+  </si>
+  <si>
+    <t>Du Toit,</t>
   </si>
 </sst>
 </file>
@@ -261,6 +328,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -562,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7A021B-F23A-0445-BE3E-AFCCAADE66BD}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,4 +980,107 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CA27B5-112E-A047-A70A-D78234E86DFB}">
+  <dimension ref="A3:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>